<commit_message>
Timesheet Stuff and Minor Changes
</commit_message>
<xml_diff>
--- a/Timesheets/kjohnson/kjohnson10.xlsx
+++ b/Timesheets/kjohnson/kjohnson10.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Senior Project - Spring / Summer 2015</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Worked on Question Tool, Bug Fixes</t>
+  </si>
+  <si>
+    <t>Total 8.5</t>
   </si>
 </sst>
 </file>
@@ -85,7 +88,7 @@
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -130,12 +133,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,7 +191,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -224,10 +221,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,7 +248,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -332,7 +325,7 @@
       <c r="D7" s="6" t="n">
         <v>0.75</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -360,7 +353,7 @@
       <c r="D9" s="6" t="n">
         <v>1.5</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -372,14 +365,16 @@
       <c r="D10" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -413,10 +408,10 @@
       <c r="E16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>